<commit_message>
database string only replacement
</commit_message>
<xml_diff>
--- a/uploads/master.xlsx
+++ b/uploads/master.xlsx
@@ -31,10 +31,10 @@
     <x:t>Erik Bridges</x:t>
   </x:si>
   <x:si>
-    <x:t>555-555-5555</x:t>
-  </x:si>
-  <x:si>
-    <x:t>$app</x:t>
+    <x:t> 555-555-555</x:t>
+  </x:si>
+  <x:si>
+    <x:t> $app</x:t>
   </x:si>
 </x:sst>
 </file>

</xml_diff>